<commit_message>
Two ways on worksheet
</commit_message>
<xml_diff>
--- a/ListCompareAlternatives.xlsx
+++ b/ListCompareAlternatives.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{FC1CC79B-2E70-42E7-82D8-14F3BAF3E3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{EF741C58-6827-4179-B245-A6CBD6F592E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>FROM:</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>Countifs</t>
   </si>
 </sst>
 </file>
@@ -1213,10 +1216,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="B2:G11"/>
+  <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1319,6 +1322,21 @@
       </c>
       <c r="G11" t="str" cm="1">
         <f t="array" ref="G11">_xlfn.LAMBDA(_xlpm.source,_xlpm.ContainedIn,_xlfn._xlws.FILTER(_xlpm.source,1-ISNUMBER(_xlfn.XMATCH(_xlpm.source, _xlpm.ContainedIn))))(D4:D9,B4:B9)</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F16" t="str" cm="1">
+        <f t="array" ref="F16">_xlfn.LAMBDA(_xlpm.Reference,_xlpm.ContainedIn,_xlfn._xlws.FILTER(_xlpm.Reference,COUNTIFS(_xlpm.ContainedIn,_xlpm.Reference)=0))(B4:B9,D4:D9)</f>
+        <v>G</v>
+      </c>
+      <c r="G16" t="str" cm="1">
+        <f t="array" ref="G16">_xlfn.LAMBDA(_xlpm.Reference,_xlpm.ContainedIn,_xlfn._xlws.FILTER(_xlpm.Reference,COUNTIFS(_xlpm.ContainedIn,_xlpm.Reference)=0))(D4:D9,B4:B9)</f>
         <v>F</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Checked out gist update
</commit_message>
<xml_diff>
--- a/ListCompareAlternatives.xlsx
+++ b/ListCompareAlternatives.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{EF741C58-6827-4179-B245-A6CBD6F592E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{6005C75F-D56B-440D-BCCD-AFBEFFD2E377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -18,6 +18,18 @@
     <sheet name="Lists" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_fBCAST">_xlfn.LAMBDA(_xlpm._nData, _xlfn.LET(_xlpm.f, _xlfn.LAMBDA(_xlpm._d, _xlfn.LET(_xlpm._c, COLUMNS(_xlpm._d) - 1, _xlfn.DROP(_xlfn.REDUCE("", _xlfn.TAKE(_xlpm._d, , 1), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, _xlfn.EXPAND(_xlpm.v, _xlpm._c, 1, _xlpm.v)))), 1))), _xlfn.HSTACK(_xlpm.f(_xlpm._nData), _xlfn.TOCOL(_xlfn.DROP(_xlpm._nData, , 1)))))</definedName>
+    <definedName name="_fCharCount">_xlfn.LAMBDA(_xlpm.s,_xlpm.c, _xlfn.LET(_xlpm.z, SUBSTITUTE(_xlpm.s, _xlpm.c, ""), LEN(_xlpm.s) - LEN(_xlpm.z)))</definedName>
+    <definedName name="_fDN">_xlfn.LAMBDA(_xlpm.arr,_xlop.ini, _xlfn.LET(_xlpm._ini, IF(_xlfn.ISOMITTED(_xlpm.ini), "", _xlpm.ini), _xlfn.SCAN(_xlpm._ini, _xlpm.arr, _xlfn.LAMBDA(_xlpm.a,_xlpm.v, IF(LEN(_xlpm.v) = 0, _xlpm.a, _xlpm.v)))))</definedName>
+    <definedName name="_fDX">_xlfn.LAMBDA(_xlpm.vlookup_value,_xlpm.vlookup_array,_xlpm.hlookup_value,_xlpm.hlookup_array,_xlpm.return_array,_xlop.if_not_found,_xlop.vmatch_mode,_xlop.vsearch_mode,_xlop.hmatch_mode,_xlop.hsearch_mode, IFERROR(INDEX(_xlpm.return_array, _xlfn.XMATCH(_xlpm.vlookup_value, _xlpm.vlookup_array, _xlpm.vmatch_mode, _xlpm.vsearch_mode), _xlfn.XMATCH(_xlpm.hlookup_value, _xlpm.hlookup_array, _xlpm.hmatch_mode, _xlpm.hsearch_mode)), IF(ISOMlTTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)))</definedName>
+    <definedName name="_fIndex">_xlfn.LAMBDA(_xlpm.d,_xlpm.r, INDEX(_xlpm.d, _xlpm.r, _xlfn.SEQUENCE(1, COLUMNS(_xlpm.d))))</definedName>
+    <definedName name="_fInterp">_xlfn.LAMBDA(_xlpm.x,_xlpm.xdat,_xlpm.ydat, _xlfn.LET(_xlpm.xmin, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.xdat, , -1), _xlpm.xmax, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.xdat, , 1), _xlpm.ymin, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.ydat, , -1), _xlpm.ymax, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.ydat, , 1), IF(_xlpm.xmin = _xlpm.xmax, _xlpm.ymin, (_xlpm.ymin * (_xlpm.xmax - _xlpm.x) + _xlpm.ymax * (_xlpm.x - _xlpm.xmin)) / (_xlpm.xmax - _xlpm.xmin))))</definedName>
+    <definedName name="_fLC">_xlfn.LAMBDA(_xlpm.Reference,_xlpm.ContainedIn, _xlfn._xlws.FILTER(_xlpm.Reference, COUNTIFS(_xlpm.ContainedIn, _xlpm.Reference) = 0))</definedName>
+    <definedName name="_fQ">_xlfn.LAMBDA(_xlpm.x, ROUNDUP(MONTH(1 &amp; _xlpm.x) / 3, 0))</definedName>
+    <definedName name="_fSUPERXLOOKUP">_xlfn.LAMBDA(_xlpm.lookup_value,_xlpm.lookup_array,_xlpm.return_array,_xlop.if_not_found,_xlop.match_mode,_xlop.search_mode, IF(COLUMNS(_xlpm.lookup_value) = 1, IFERROR(INDEX(_xlpm.return_array, _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode), _xlfn.SEQUENCE(1, COLUMNS(_xlpm.return_array))), IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)), IFERROR(INDEX(_xlpm.return_array, _xlfn.SEQUENCE(ROWS(_xlpm.return_array)), _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode)), IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found))))</definedName>
+    <definedName name="_fUP">_xlfn.LAMBDA(_xlpm.arr,_xlop.ini, _xlfn.LET(_xlpm._f, _xlfn.LAMBDA(_xlpm.z, INDEX(_xlpm.z, _xlfn.SEQUENCE(ROWS(_xlpm.z), 1, ROWS(_xlpm.z), -1))), _xlpm._arr, _xlpm._f(_xlpm.arr), _xlpm._ini, IF(_xlfn.ISOMITTED(_xlpm.ini), "", _xlpm.ini), _xlpm._f(_xlfn.SCAN(_xlpm._ini, _xlpm._arr, _xlfn.LAMBDA(_xlpm.a,_xlpm.v, IF(LEN(_xlpm.v) = 0, _xlpm.a, _xlpm.v))))))</definedName>
+    <definedName name="DDL">_xlfn.LAMBDA(_xlpm.range,_xlop.lookup1,_xlop.lookup2,_xlop.lookup3,_xlop.lookup4,_xlop.lookup5,_xlop.lookup6,_xlop.lookup7,_xlop.lookup8,_xlop.lookup9,_xlop.lookup10, _xlfn.LET(_xlpm._s, "%^&amp;&amp;@", _xlpm.lookupValue, _xlpm.lookup1 &amp; _xlpm._s &amp; _xlpm.lookup2 &amp; _xlpm._s &amp; _xlpm.lookup3 &amp; _xlpm._s &amp; _xlpm.lookup4 &amp; _xlpm._s &amp; _xlpm.lookup5 &amp; _xlpm._s &amp; _xlpm.lookup6 &amp; _xlpm._s &amp; _xlpm.lookup7 &amp; _xlpm._s &amp; _xlpm.lookup8 &amp; _xlpm._s &amp; _xlpm.lookup9 &amp; _xlpm._s &amp; _xlpm.lookup10, _xlpm.levelIndex, IFERROR(ROWS(_xlfn.TEXTSPLIT(_xlpm.lookupValue, , _xlpm._s, TRUE())), 0) + 1, _xlpm.lookupArray, _xlfn.BYROW(_xlfn.EXPAND(_xlfn.CHOOSECOLS(_xlpm.range, _xlfn.SEQUENCE(1, _xlpm.levelIndex - 1)), , 10, ""), _xlfn.LAMBDA(_xlpm.row, _xlfn.TEXTJOIN(_xlpm._s, FALSE, _xlpm.row))), _xlpm.returnRange, INDEX(_xlpm.range, 0, _xlpm.levelIndex), _xlpm.result, IF(_xlfn.ISOMITTED(_xlpm.lookup1) * _xlpm.levelIndex = 1, _xlpm.returnRange, _xlfn.XLOOKUP(_xlpm.lookupValue, _xlpm.lookupArray, _xlpm.returnRange):_xlfn.XLOOKUP(_xlpm.lookupValue, _xlpm.lookupArray, _xlpm.returnRange, , , -1)), _xlpm.result))</definedName>
+    <definedName name="DDLSorter">_xlfn.LAMBDA(_xlpm.Range,_xlop.SortOrder, _xlfn._xlws.SORT(_xlpm.Range, _xlfn.SEQUENCE(, COLUMNS(_xlpm.Range)), _xlpm.SortOrder))</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1211,15 +1223,44 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{A17A1725-49BE-48F8-B655-071C951127EE}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{29F40CFD-BD46-4D3D-A633-BA05AE20C3AB}&quot;}"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="B2:G16"/>
+  <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1337,6 +1378,16 @@
       </c>
       <c r="G16" t="str" cm="1">
         <f t="array" ref="G16">_xlfn.LAMBDA(_xlpm.Reference,_xlpm.ContainedIn,_xlfn._xlws.FILTER(_xlpm.Reference,COUNTIFS(_xlpm.ContainedIn,_xlpm.Reference)=0))(D4:D9,B4:B9)</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" t="str" cm="1">
+        <f t="array" ref="F20">_fLC(B4:B9,D4:D9)</f>
+        <v>G</v>
+      </c>
+      <c r="G20" t="str" cm="1">
+        <f t="array" ref="G20">_fLC(D4:D9,B4:B9)</f>
         <v>F</v>
       </c>
     </row>
@@ -1686,4 +1737,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AXABuAC8ALwAgAEcAZQBuAGUAcgBhAHQAZQAgAGEAbgAgAGkAbgBkAGUAeAAgAGMAbwBsAHUAbQBuACAAdABoAGUAIABoAGUAaQBnAGgAdAAgAG8AZgAgAHQAaABlACAAZABhAHQAYQAgAGQAXABuAF8AZgBJAG4AZABlAHgAPQBMAEEATQBCAEQAQQAoAGQALAByACwASQBOAEQARQBYACgAZAAsAHIALABTAEUAUQBVAEUATgBDAEUAKAAxACwAQwBPAEwAVQBNAE4AUwAoAGQAKQApACkAKQA7AFwAbgAvAC8AIABTAHUAcABlAHIAWABMAE8ATwBLAFUAUABcAG4AXwBmAFMAVQBQAEUAUgBYAEwATwBPAEsAVQBQAD0ATABBAE0AQgBEAEEAKABsAG8AbwBrAHUAcABfAHYAYQBsAHUAZQAsAGwAbwBvAGsAdQBwAF8AYQByAHIAYQB5ACwAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkALABbAGkAZgBfAG4AbwB0AF8AZgBvAHUAbgBkAF0ALABbAG0AYQB0AGMAaABfAG0AbwBkAGUAXQAsAFsAcwBlAGEAcgBjAGgAXwBtAG8AZABlAF0ALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAEMATwBMAFUATQBOAFMAKABsAG8AbwBrAHUAcABfAHYAYQBsAHUAZQApACAAPQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgBFAFIAUgBPAFIAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABYAE0AQQBUAEMASAAoAGwAbwBvAGsAdQBwAF8AdgBhAGwAdQBlACwAIABsAG8AbwBrAHUAcABfAGEAcgByAGEAeQAsACAAbQBhAHQAYwBoAF8AbQBvAGQAZQAsACAAcwBlAGEAcgBjAGgAXwBtAG8AZABlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAEUAUQBVAEUATgBDAEUAKAAxACwAIABDAE8ATABVAE0ATgBTACgAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAaQBmAF8AbgBvAHQAXwBmAG8AdQBuAGQAKQAsACAATgBBACgAKQAsACAAaQBmAF8AbgBvAHQAXwBmAG8AdQBuAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgBFAFIAUgBPAFIAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAEUAUQBVAEUATgBDAEUAKABSAE8AVwBTACgAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAWABNAEEAVABDAEgAKABsAG8AbwBrAHUAcABfAHYAYQBsAHUAZQAsACAAbABvAG8AawB1AHAAXwBhAHIAcgBhAHkALAAgAG0AYQB0AGMAaABfAG0AbwBkAGUALAAgAHMAZQBhAHIAYwBoAF8AbQBvAGQAZQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAaQBmAF8AbgBvAHQAXwBmAG8AdQBuAGQAKQAsACAATgBBACgAKQAsACAAaQBmAF8AbgBvAHQAXwBmAG8AdQBuAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAvACAATABpAG4AZQBhAHIAIABJAG4AdABlAHIAcABvAGwAYQB0AGkAbwBuACAARgBvAHIAbQB1AGwAYQBcAG4AXwBmAEkAbgB0AGUAcgBwAD0ATABBAE0AQgBEAEEAKAB4ACwAeABkAGEAdAAsAHkAZABhAHQALABcAG4AIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgAHgAbQBpAG4ALAAgAFgATABPAE8ASwBVAFAAKAB4ACwAeABkAGEAdAAsAHgAZABhAHQALAAsAC0AMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgAHgAbQBhAHgALAAgAFgATABPAE8ASwBVAFAAKAB4ACwAeABkAGEAdAAsAHgAZABhAHQALAAsADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAB5AG0AaQBuACwAIABYAEwATwBPAEsAVQBQACgAeAAsAHgAZABhAHQALAB5AGQAYQB0ACwALAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAB5AG0AYQB4ACwAIABYAEwATwBPAEsAVQBQACgAeAAsAHgAZABhAHQALAB5AGQAYQB0ACwALAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAASQBGACgAeABtAGkAbgA9AHgAbQBhAHgALAB5AG0AaQBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAeQBtAGkAbgAqACgAeABtAGEAeAAtAHgAKQArAHkAbQBhAHgAKgAoAHgALQB4AG0AaQBuACkAKQAvACgAeABtAGEAeAAtAHgAbQBpAG4AKQApAFwAbgAgACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAvACAAQwBvAHUAbgB0ACAAYQAgAHMAcABlAGMAaQBmAGkAYwAgAGMAaABhAHIAYQBjAHQAZQByACAAaQBuACAAYQAgAHMAdAByAGkAbgBnAFwAbgBfAGYAQwBoAGEAcgBDAG8AdQBuAHQAPQBMAEEATQBCAEQAQQAoAHMALABjACwATABFAFQAKAB6ACwAUwBVAEIAUwBUAEkAVABVAFQARQAoAHMALABjACwAXAAiAFwAIgApACwATABFAE4AKABzACkALQBMAEUATgAoAHoAKQApACkAOwBcAG4AXABuAC8ALwAgAEYAaQBsAGwAIABEAG8AdwBuAFwAbgBfAGYARABOAD0ATABBAE0AQgBEAEEAKABhAHIAcgAsAFsAaQBuAGkAXQAsAFwAbgBMAEUAVAAoAFwAbgBfAGkAbgBpACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGkAbgBpACkALABcACIAXAAiACwAaQBuAGkAKQAsAFwAbgBTAEMAQQBOACgAXwBpAG4AaQAsAGEAcgByACwATABBAE0AQgBEAEEAKABhACwAdgAsAEkARgAoAEwARQBOACgAdgApAD0AMAAsAGEALAB2ACkAKQApAFwAbgApAFwAbgApADsAXABuAFwAbgAvAC8AIABGAGkAbABsACAAVQBwAFwAbgBfAGYAVQBQAD0ATABBAE0AQgBEAEEAKABhAHIAcgAsAFsAaQBuAGkAXQAsAFwAbgBMAEUAVAAoAFwAbgBfAGYALABMAEEATQBCAEQAQQAoAHoALABJAE4ARABFAFgAKAB6ACwAUwBFAFEAVQBFAE4AQwBFACgAUgBPAFcAUwAoAHoAKQAsADEALABSAE8AVwBTACgAegApACwALQAxACkAKQApACwAXABuAF8AYQByAHIALAAgAF8AZgAoAGEAcgByACkALABcAG4AXwBpAG4AaQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABpAG4AaQApACwAXAAiAFwAIgAsAGkAbgBpACkALABcAG4AXwBmACgAUwBDAEEATgAoAF8AaQBuAGkALABfAGEAcgByACwATABBAE0AQgBEAEEAKABhACwAdgAsAEkARgAoAEwARQBOACgAdgApAD0AMAAsAGEALAB2ACkAKQApACkAXABuACkAXABuACkAOwBcAG4AXABuAC8ALwAgAEIAcgBvAGEAZABjAGEAcwB0ACAAZgBpAHIAcwB0ACAAYwBvAGwAdQBtAG4AXABuAF8AZgBCAEMAQQBTAFQAPQBMAEEATQBCAEQAQQAoAF8AbgBEAGEAdABhACwATABFAFQAKABmACwAIABMAEEATQBCAEQAQQAoAF8AZAAsAEwARQBUACgAXwBjACwAQwBPAEwAVQBNAE4AUwAoAF8AZAApAC0AMQAsAEQAUgBPAFAAKABSAEUARABVAEMARQAoAFwAIgBcACIALABUAEEASwBFACgAXwBkACwALAAxACkALABMAEEATQBCAEQAQQAoAGEALAB2ACwAVgBTAFQAQQBDAEsAKABhACwARQBYAFAAQQBOAEQAKAB2ACwAXwBjACwAMQAsAHYAKQApACkAKQAsADEAKQApACkALABcAG4AIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAZgAoAF8AbgBEAGEAdABhACkALABUAE8AQwBPAEwAKABEAFIATwBQACgAXwBuAEQAYQB0AGEALAAsADEAKQApACkAXABuACkAKQA7AFwAbgBcAG4ALwAvACAATQBhAHIAawAgAFAAcgBvAGMAdABvAHIAIABEAEQATAAgAGYAdQBuAGMAdABpAG8AbgBcAG4ARABEAEwAPQBMAEEATQBCAEQAQQAoAHIAYQBuAGcAZQAsAFsAbABvAG8AawB1AHAAMQBdACwAWwBsAG8AbwBrAHUAcAAyAF0ALABbAGwAbwBvAGsAdQBwADMAXQAsAFsAbABvAG8AawB1AHAANABdACwAWwBsAG8AbwBrAHUAcAA1AF0ALABbAGwAbwBvAGsAdQBwADYAXQAsAFsAbABvAG8AawB1AHAANwBdACwAWwBsAG8AbwBrAHUAcAA4AF0ALABbAGwAbwBvAGsAdQBwADkAXQAsAFsAbABvAG8AawB1AHAAMQAwAF0ALABcAG4ATABFAFQAKABcAG4AXwBzACwAIABcACIAJQBeACYAJgBAAFwAIgAsACAAXABuAGwAbwBvAGsAdQBwAFYAYQBsAHUAZQAsACAAbABvAG8AawB1AHAAMQAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAAMgAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAAMwAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAANAAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAANQAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAANgAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAANwAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAAOAAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAAOQAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAAMQAwACwAXABuAGwAZQB2AGUAbABJAG4AZABlAHgALAAgAEkARgBFAFIAUgBPAFIAKABSAE8AVwBTACgAVABFAFgAVABTAFAATABJAFQAKABsAG8AbwBrAHUAcABWAGEAbAB1AGUALAAgACwAIABfAHMALAAgAFQAUgBVAEUAKAApACkAKQAsACAAMAApACAAKwAgADEALAAgAFwAbgBsAG8AbwBrAHUAcABBAHIAcgBhAHkALAAgAEIAWQBSAE8AVwAoAEUAWABQAEEATgBEACgAQwBIAE8ATwBTAEUAQwBPAEwAUwAoAHIAYQBuAGcAZQAsACAAUwBFAFEAVQBFAE4AQwBFACgAMQAsACAAbABlAHYAZQBsAEkAbgBkAGUAeAAgAC0AIAAxACkAKQAsACAALAAgADEAMAAsACAAXAAiAFwAIgApACwAIABMAEEATQBCAEQAQQAoAHIAbwB3ACwAIABUAEUAWABUAEoATwBJAE4AKABfAHMALAAgAEYAQQBMAFMARQAsACAAcgBvAHcAKQApACkALABcAG4AcgBlAHQAdQByAG4AUgBhAG4AZwBlACwAIABJAE4ARABFAFgAKAByAGEAbgBnAGUALAAgADAALAAgAGwAZQB2AGUAbABJAG4AZABlAHgAKQAsACAAXABuAHIAZQBzAHUAbAB0ACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGwAbwBvAGsAdQBwADEAKQAgACoAIABsAGUAdgBlAGwASQBuAGQAZQB4ACAAPQAgADEALAAgAHIAZQB0AHUAcgBuAFIAYQBuAGcAZQAsACAAWABMAE8ATwBLAFUAUAAoAGwAbwBvAGsAdQBwAFYAYQBsAHUAZQAsACAAbABvAG8AawB1AHAAQQByAHIAYQB5ACwAIAByAGUAdAB1AHIAbgBSAGEAbgBnAGUAKQA6AFgATABPAE8ASwBVAFAAKABsAG8AbwBrAHUAcABWAGEAbAB1AGUALAAgAGwAbwBvAGsAdQBwAEEAcgByAGEAeQAsACAAcgBlAHQAdQByAG4AUgBhAG4AZwBlACwAIAAsACAALAAgAC0AMQApACkALABcAG4AcgBlAHMAdQBsAHQAKQApADsAXABuAFwAbgAvAC8AIABNAGEAcgBrACAAUAByAG8AYwB0AG8AcgAgAEQARABMAFMAbwByAHQAZQByACAAZgB1AG4AYwB0AGkAbwBuAFwAbgBcAG4ARABEAEwAUwBvAHIAdABlAHIAPQBMAEEATQBCAEQAQQAoAFIAYQBuAGcAZQAsAFsAUwBvAHIAdABPAHIAZABlAHIAXQAsAFMATwBSAFQAKABSAGEAbgBnAGUALAAgAFMARQBRAFUARQBOAEMARQAoACwAIABDAE8ATABVAE0ATgBTACgAUgBhAG4AZwBlACkAKQAsACAAUwBvAHIAdABPAHIAZABlAHIAKQApADsAXABuAFwAbgAvAC8AIABEAG8AdQBiAGwAZQAgAFgATABPAE8ASwBVAFAAXABuAFwAbgBfAGYARABYAD0ATABBAE0AQgBEAEEAKAB2AGwAbwBvAGsAdQBwAF8AdgBhAGwAdQBlACwAdgBsAG8AbwBrAHUAcABfAGEAcgByAGEAeQAsAGgAbABvAG8AawB1AHAAXwB2AGEAbAB1AGUALABoAGwAbwBvAGsAdQBwAF8AYQByAHIAYQB5ACwAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkALABbAGkAZgBfAG4AbwB0AF8AZgBvAHUAbgBkAF0ALABbAHYAbQBhAHQAYwBoAF8AbQBvAGQAZQBdACwAWwB2AHMAZQBhAHIAYwBoAF8AbQBvAGQAZQBdACwAWwBoAG0AYQB0AGMAaABfAG0AbwBkAGUAXQAsAFsAaABzAGUAYQByAGMAaABfAG0AbwBkAGUAXQAsACAASQBGAEUAUgBSAE8AUgAoACAASQBOAEQARQBYACgAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkALABYAE0AQQBUAEMASAAoAHYAbABvAG8AawB1AHAAXwB2AGEAbAB1AGUALAB2AGwAbwBvAGsAdQBwAF8AYQByAHIAYQB5ACwAdgBtAGEAdABjAGgAXwBtAG8AZABlACwAdgBzAGUAYQByAGMAaABfAG0AbwBkAGUAKQAsAFgATQBBAFQAQwBIACgAaABsAG8AbwBrAHUAcABfAHYAYQBsAHUAZQAsAGgAbABvAG8AawB1AHAAXwBhAHIAcgBhAHkALABoAG0AYQB0AGMAaABfAG0AbwBkAGUALABoAHMAZQBhAHIAYwBoAF8AbQBvAGQAZQApACkALAAgAEkARgAoAEkAUwBPAE0AbABUAFQARQBEACgAaQBmAF8AbgBvAHQAXwBmAG8AdQBuAGQAKQAsAE4AQQAoACkALABpAGYAXwBuAG8AdABfAGYAbwB1AG4AZAApACkAKQA7AFwAbgBcAG4ALwAvACAAUQB1AGEAcgB0AGUAcgAgAGYAcgBvAG0AIABNAG8AbgB0AGgAIABBAGIAYgByAGUAdgBpAGEAdABpAG8AbgBcAG4AXABuAF8AZgBRAD0ATABBAE0AQgBEAEEAKAB4ACwAUgBPAFUATgBEAFUAUAAoAE0ATwBOAFQASAAoADEAJgB4ACkALwAzACwAMAApACkAOwBcAG4AXABuAC8ALwBMAGkAcwB0ACAAQwBvAG0AcABhAHIAZQBcAG4AXABuAF8AZgBMAEMAPQBMAEEATQBCAEQAQQAoAFIAZQBmAGUAcgBlAG4AYwBlACwAQwBvAG4AdABhAGkAbgBlAGQASQBuACwARgBJAEwAVABFAFIAKABSAGUAZgBlAHIAZQBuAGMAZQAsAEMATwBVAE4AVABJAEYAUwAoAEMAbwBuAHQAYQBpAG4AZQBkAEkAbgAsAFIAZQBmAGUAcgBlAG4AYwBlACkAPQAwACkAKQA7ACIAfQBdACwAIgBwAHIAbwBqAGUAYwB0AE4AYQBtAGUAcwAiADoAWwAiAF8AZgBJAG4AZABlAHgAIgAsACIAXwBmAFMAVQBQAEUAUgBYAEwATwBPAEsAVQBQACIALAAiAF8AZgBJAG4AdABlAHIAcAAiACwAIgBfAGYAQwBoAGEAcgBDAG8AdQBuAHQAIgAsACIAXwBmAEQATgAiACwAIgBfAGYAVQBQACIALAAiAF8AZgBCAEMAQQBTAFQAIgAsACIARABEAEwAIgAsACIARABEAEwAUwBvAHIAdABlAHIAIgAsACIAXwBmAEQAWAAiACwAIgBfAGYAUQAiACwAIgBfAGYATABDACIAXQAsACIAbABvAGMAYQBsAGUAIgA6AHsAIgBsAGkAcwB0AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAcgBvAHcAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBjAG8AbAB1AG0AbgBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAdABoAG8AdQBzAGEAbgBkAHMAUABvAHMAaQB0AGkAbwBuAHMAIgA6AFsAMwBdACwAIgBkAGUAYwBpAG0AYQBsAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiAC4AIgAsACIAZABhAHQAZQBPAHIAZABlAHIAIgA6ACIARABNAFkAIgAsACIAYwB1AHIAcgBlAG4AYwB5AFMAeQBtAGIAbwBsACIAOgAiACQAIgAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbABMAGUAYQBkACIAOgB0AHIAdQBlACwAIgBpAHMAQwB1AHIAcgBlAG4AYwB5AFMAZQBwAEIAeQBTAHAAYQBjAGUAIgA6AGYAYQBsAHMAZQAsACIAcgBvAHcATABlAHQAdABlAHIAIgA6ACIAUgAiACwAIgBjAG8AbAB1AG0AbgBMAGUAdAB0AGUAcgAiADoAIgBDACIALAAiAHIAYwBMAGUAZgB0AEIAcgBhAGMAawBlAHQAIgA6ACIAWwAiACwAIgByAGMAUgBpAGcAaAB0AEIAcgBhAGMAawBlAHQAIgA6ACIAXQAiACwAIgBzAHQAYQB0AGUAbQBlAG4AdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgA7ACIALAAiAGwAbwBjAGEAbABlAE4AYQBtAGUAIgA6ACIAZQBuAC0AdQBzACIAfQB9AA==</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F40CFD-BD46-4D3D-A633-BA05AE20C3AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>